<commit_message>
Updated Job Search File
</commit_message>
<xml_diff>
--- a/Job Search Record Template.xlsx
+++ b/Job Search Record Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/new/Desktop/Useful information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE873A29-61F2-604C-9B87-EA6DD48B302B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E877D23-18A4-5C47-8D80-96971A371C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19180" xr2:uid="{9EDEA7B2-21B2-6E4D-B3E8-2A2EBC0C752F}"/>
   </bookViews>
@@ -1267,7 +1267,7 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1459,7 +1459,7 @@
         <v>44637</v>
       </c>
       <c r="G9" s="10">
-        <v>44649</v>
+        <v>44639</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>